<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-13.xlsx - 2026-01-13T10:20:51.053Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-13.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-13.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,51 +449,95 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 10:09</v>
+        <v>2026-01-13 10:20</v>
       </c>
       <c r="C2" t="str">
-        <v>Anuradha N</v>
+        <v>Pooja</v>
       </c>
       <c r="D2" t="str">
-        <v>B 304</v>
+        <v>A 1608</v>
       </c>
       <c r="E2" t="str">
         <v/>
       </c>
       <c r="F2" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G2">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H2" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I2" t="str">
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K2" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L2" t="str">
+        <v/>
+      </c>
+      <c r="M2" t="str">
+        <v/>
+      </c>
+      <c r="N2" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="str">
+        <v>2026-01-13 10:09</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Anuradha N</v>
+      </c>
+      <c r="D3" t="str">
+        <v>B 304</v>
+      </c>
+      <c r="E3" t="str">
+        <v/>
+      </c>
+      <c r="F3" t="str">
+        <v>Til Poli x1</v>
+      </c>
+      <c r="G3">
+        <v>30</v>
+      </c>
+      <c r="H3" t="str">
+        <v>COOKING</v>
+      </c>
+      <c r="I3" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J3" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K2" t="str">
+      <c r="K3" t="str">
         <v>16:45</v>
       </c>
-      <c r="L2" t="str">
-        <v/>
-      </c>
-      <c r="M2" t="str">
-        <v/>
-      </c>
-      <c r="N2" t="str">
+      <c r="L3" t="str">
+        <v/>
+      </c>
+      <c r="M3" t="str">
+        <v/>
+      </c>
+      <c r="N3" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N3"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -533,7 +577,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -542,13 +586,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-13.xlsx - 2026-01-13T11:15:14.801Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-13.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-13.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,25 +449,25 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C2" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D2" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E2" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F2" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G2">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -479,7 +479,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K2" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -493,51 +493,95 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 10:09</v>
+        <v>2026-01-13 10:20</v>
       </c>
       <c r="C3" t="str">
-        <v>Anuradha N</v>
+        <v>Pooja</v>
       </c>
       <c r="D3" t="str">
-        <v>B 304</v>
+        <v>A 1608</v>
       </c>
       <c r="E3" t="str">
         <v/>
       </c>
       <c r="F3" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G3">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H3" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I3" t="str">
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K3" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L3" t="str">
+        <v/>
+      </c>
+      <c r="M3" t="str">
+        <v/>
+      </c>
+      <c r="N3" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="str">
+        <v>2026-01-13 10:09</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Anuradha N</v>
+      </c>
+      <c r="D4" t="str">
+        <v>B 304</v>
+      </c>
+      <c r="E4" t="str">
+        <v/>
+      </c>
+      <c r="F4" t="str">
+        <v>Til Poli x1</v>
+      </c>
+      <c r="G4">
+        <v>30</v>
+      </c>
+      <c r="H4" t="str">
+        <v>COOKING</v>
+      </c>
+      <c r="I4" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J4" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K3" t="str">
+      <c r="K4" t="str">
         <v>16:45</v>
       </c>
-      <c r="L3" t="str">
-        <v/>
-      </c>
-      <c r="M3" t="str">
-        <v/>
-      </c>
-      <c r="N3" t="str">
+      <c r="L4" t="str">
+        <v/>
+      </c>
+      <c r="M4" t="str">
+        <v/>
+      </c>
+      <c r="N4" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N4"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -577,7 +621,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -586,13 +630,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>45</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-13.xlsx - 2026-01-13T16:39:10.100Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-13.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-13.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,25 +449,25 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 11:15</v>
+        <v>2026-01-13 16:39</v>
       </c>
       <c r="C2" t="str">
-        <v>Ajay Dwarkunde</v>
+        <v>Pooja</v>
       </c>
       <c r="D2" t="str">
-        <v>b-703</v>
+        <v>A1608</v>
       </c>
       <c r="E2" t="str">
-        <v>8087172173</v>
+        <v>9096648553</v>
       </c>
       <c r="F2" t="str">
-        <v>Pohe x1</v>
+        <v>Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G2">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -476,10 +476,10 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K2" t="str">
-        <v>18:50</v>
+        <v>22:09</v>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -493,25 +493,25 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C3" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D3" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E3" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F3" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G3">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H3" t="str">
         <v>NEW</v>
@@ -523,7 +523,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K3" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -537,51 +537,95 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 10:09</v>
+        <v>2026-01-13 10:20</v>
       </c>
       <c r="C4" t="str">
-        <v>Anuradha N</v>
+        <v>Pooja</v>
       </c>
       <c r="D4" t="str">
-        <v>B 304</v>
+        <v>A 1608</v>
       </c>
       <c r="E4" t="str">
         <v/>
       </c>
       <c r="F4" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G4">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H4" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I4" t="str">
         <v>PENDING</v>
       </c>
       <c r="J4" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K4" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L4" t="str">
+        <v/>
+      </c>
+      <c r="M4" t="str">
+        <v/>
+      </c>
+      <c r="N4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="str">
+        <v>2026-01-13 10:09</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Anuradha N</v>
+      </c>
+      <c r="D5" t="str">
+        <v>B 304</v>
+      </c>
+      <c r="E5" t="str">
+        <v/>
+      </c>
+      <c r="F5" t="str">
+        <v>Til Poli x1</v>
+      </c>
+      <c r="G5">
+        <v>30</v>
+      </c>
+      <c r="H5" t="str">
+        <v>COOKING</v>
+      </c>
+      <c r="I5" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J5" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K4" t="str">
+      <c r="K5" t="str">
         <v>16:45</v>
       </c>
-      <c r="L4" t="str">
-        <v/>
-      </c>
-      <c r="M4" t="str">
-        <v/>
-      </c>
-      <c r="N4" t="str">
+      <c r="L5" t="str">
+        <v/>
+      </c>
+      <c r="M5" t="str">
+        <v/>
+      </c>
+      <c r="N5" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N5"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -621,7 +665,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -630,13 +674,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>75</v>
+        <v>135</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>75</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-13.xlsx - 2026-01-13T16:40:54.941Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-13.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-13.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,25 +449,25 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 16:39</v>
+        <v>2026-01-13 16:40</v>
       </c>
       <c r="C2" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D2" t="str">
-        <v>A1608</v>
+        <v>A-1608</v>
       </c>
       <c r="E2" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F2" t="str">
-        <v>Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G2">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -479,7 +479,7 @@
         <v>2026-01-14</v>
       </c>
       <c r="K2" t="str">
-        <v>22:09</v>
+        <v>10:00</v>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -493,25 +493,25 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 11:15</v>
+        <v>2026-01-13 16:39</v>
       </c>
       <c r="C3" t="str">
-        <v>Ajay Dwarkunde</v>
+        <v>Pooja</v>
       </c>
       <c r="D3" t="str">
-        <v>b-703</v>
+        <v>A1608</v>
       </c>
       <c r="E3" t="str">
-        <v>8087172173</v>
+        <v>9096648553</v>
       </c>
       <c r="F3" t="str">
-        <v>Pohe x1</v>
+        <v>Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G3">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H3" t="str">
         <v>NEW</v>
@@ -520,10 +520,10 @@
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K3" t="str">
-        <v>18:50</v>
+        <v>22:09</v>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -537,25 +537,25 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C4" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D4" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E4" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F4" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G4">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H4" t="str">
         <v>NEW</v>
@@ -567,7 +567,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K4" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -581,51 +581,95 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-13 10:09</v>
+        <v>2026-01-13 10:20</v>
       </c>
       <c r="C5" t="str">
-        <v>Anuradha N</v>
+        <v>Pooja</v>
       </c>
       <c r="D5" t="str">
-        <v>B 304</v>
+        <v>A 1608</v>
       </c>
       <c r="E5" t="str">
         <v/>
       </c>
       <c r="F5" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G5">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H5" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I5" t="str">
         <v>PENDING</v>
       </c>
       <c r="J5" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K5" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L5" t="str">
+        <v/>
+      </c>
+      <c r="M5" t="str">
+        <v/>
+      </c>
+      <c r="N5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="str">
+        <v>2026-01-13 10:09</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Anuradha N</v>
+      </c>
+      <c r="D6" t="str">
+        <v>B 304</v>
+      </c>
+      <c r="E6" t="str">
+        <v/>
+      </c>
+      <c r="F6" t="str">
+        <v>Til Poli x1</v>
+      </c>
+      <c r="G6">
+        <v>30</v>
+      </c>
+      <c r="H6" t="str">
+        <v>COOKING</v>
+      </c>
+      <c r="I6" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J6" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K5" t="str">
+      <c r="K6" t="str">
         <v>16:45</v>
       </c>
-      <c r="L5" t="str">
-        <v/>
-      </c>
-      <c r="M5" t="str">
-        <v/>
-      </c>
-      <c r="N5" t="str">
+      <c r="L6" t="str">
+        <v/>
+      </c>
+      <c r="M6" t="str">
+        <v/>
+      </c>
+      <c r="N6" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N6"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -665,7 +709,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -674,13 +718,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>135</v>
+        <v>165</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>135</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-13.xlsx - 2026-01-13T16:41:28.325Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-13.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-13.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,25 +449,25 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 16:40</v>
+        <v>2026-01-13 16:41</v>
       </c>
       <c r="C2" t="str">
-        <v>Sagar Borse</v>
+        <v>Pooja</v>
       </c>
       <c r="D2" t="str">
-        <v>A-1608</v>
+        <v>saf</v>
       </c>
       <c r="E2" t="str">
-        <v>7588930329</v>
+        <v>9096648553</v>
       </c>
       <c r="F2" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G2">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -476,10 +476,10 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K2" t="str">
-        <v>10:00</v>
+        <v>10:12</v>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -493,25 +493,25 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 16:39</v>
+        <v>2026-01-13 16:40</v>
       </c>
       <c r="C3" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D3" t="str">
-        <v>A1608</v>
+        <v>A-1608</v>
       </c>
       <c r="E3" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F3" t="str">
-        <v>Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G3">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H3" t="str">
         <v>NEW</v>
@@ -523,7 +523,7 @@
         <v>2026-01-14</v>
       </c>
       <c r="K3" t="str">
-        <v>22:09</v>
+        <v>10:00</v>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -537,25 +537,25 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 11:15</v>
+        <v>2026-01-13 16:39</v>
       </c>
       <c r="C4" t="str">
-        <v>Ajay Dwarkunde</v>
+        <v>Pooja</v>
       </c>
       <c r="D4" t="str">
-        <v>b-703</v>
+        <v>A1608</v>
       </c>
       <c r="E4" t="str">
-        <v>8087172173</v>
+        <v>9096648553</v>
       </c>
       <c r="F4" t="str">
-        <v>Pohe x1</v>
+        <v>Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G4">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H4" t="str">
         <v>NEW</v>
@@ -564,10 +564,10 @@
         <v>PENDING</v>
       </c>
       <c r="J4" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K4" t="str">
-        <v>18:50</v>
+        <v>22:09</v>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -581,25 +581,25 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C5" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D5" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E5" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F5" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G5">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H5" t="str">
         <v>NEW</v>
@@ -611,7 +611,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K5" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -625,51 +625,95 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-13 10:09</v>
+        <v>2026-01-13 10:20</v>
       </c>
       <c r="C6" t="str">
-        <v>Anuradha N</v>
+        <v>Pooja</v>
       </c>
       <c r="D6" t="str">
-        <v>B 304</v>
+        <v>A 1608</v>
       </c>
       <c r="E6" t="str">
         <v/>
       </c>
       <c r="F6" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G6">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H6" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I6" t="str">
         <v>PENDING</v>
       </c>
       <c r="J6" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K6" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L6" t="str">
+        <v/>
+      </c>
+      <c r="M6" t="str">
+        <v/>
+      </c>
+      <c r="N6" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="str">
+        <v>2026-01-13 10:09</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Anuradha N</v>
+      </c>
+      <c r="D7" t="str">
+        <v>B 304</v>
+      </c>
+      <c r="E7" t="str">
+        <v/>
+      </c>
+      <c r="F7" t="str">
+        <v>Til Poli x1</v>
+      </c>
+      <c r="G7">
+        <v>30</v>
+      </c>
+      <c r="H7" t="str">
+        <v>COOKING</v>
+      </c>
+      <c r="I7" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J7" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K6" t="str">
+      <c r="K7" t="str">
         <v>16:45</v>
       </c>
-      <c r="L6" t="str">
-        <v/>
-      </c>
-      <c r="M6" t="str">
-        <v/>
-      </c>
-      <c r="N6" t="str">
+      <c r="L7" t="str">
+        <v/>
+      </c>
+      <c r="M7" t="str">
+        <v/>
+      </c>
+      <c r="N7" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N7"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -709,7 +753,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -718,13 +762,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>165</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-13.xlsx - 2026-01-13T16:54:52.416Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-13.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-13.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,16 +449,16 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 16:41</v>
+        <v>2026-01-13 16:54</v>
       </c>
       <c r="C2" t="str">
         <v>Pooja</v>
       </c>
       <c r="D2" t="str">
-        <v>saf</v>
+        <v>a14</v>
       </c>
       <c r="E2" t="str">
         <v>9096648553</v>
@@ -476,10 +476,10 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-15</v>
+        <v/>
       </c>
       <c r="K2" t="str">
-        <v>10:12</v>
+        <v/>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -493,25 +493,25 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 16:40</v>
+        <v>2026-01-13 16:41</v>
       </c>
       <c r="C3" t="str">
-        <v>Sagar Borse</v>
+        <v>Pooja</v>
       </c>
       <c r="D3" t="str">
-        <v>A-1608</v>
+        <v>saf</v>
       </c>
       <c r="E3" t="str">
-        <v>7588930329</v>
+        <v>9096648553</v>
       </c>
       <c r="F3" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G3">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H3" t="str">
         <v>NEW</v>
@@ -520,10 +520,10 @@
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K3" t="str">
-        <v>10:00</v>
+        <v>10:12</v>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -537,25 +537,25 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 16:39</v>
+        <v>2026-01-13 16:40</v>
       </c>
       <c r="C4" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D4" t="str">
-        <v>A1608</v>
+        <v>A-1608</v>
       </c>
       <c r="E4" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F4" t="str">
-        <v>Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G4">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H4" t="str">
         <v>NEW</v>
@@ -567,7 +567,7 @@
         <v>2026-01-14</v>
       </c>
       <c r="K4" t="str">
-        <v>22:09</v>
+        <v>10:00</v>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -581,25 +581,25 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-13 11:15</v>
+        <v>2026-01-13 16:39</v>
       </c>
       <c r="C5" t="str">
-        <v>Ajay Dwarkunde</v>
+        <v>Pooja</v>
       </c>
       <c r="D5" t="str">
-        <v>b-703</v>
+        <v>A1608</v>
       </c>
       <c r="E5" t="str">
-        <v>8087172173</v>
+        <v>9096648553</v>
       </c>
       <c r="F5" t="str">
-        <v>Pohe x1</v>
+        <v>Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G5">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H5" t="str">
         <v>NEW</v>
@@ -608,10 +608,10 @@
         <v>PENDING</v>
       </c>
       <c r="J5" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K5" t="str">
-        <v>18:50</v>
+        <v>22:09</v>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -625,25 +625,25 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C6" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D6" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E6" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F6" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G6">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H6" t="str">
         <v>NEW</v>
@@ -655,7 +655,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K6" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L6" t="str">
         <v/>
@@ -669,51 +669,95 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-13 10:09</v>
+        <v>2026-01-13 10:20</v>
       </c>
       <c r="C7" t="str">
-        <v>Anuradha N</v>
+        <v>Pooja</v>
       </c>
       <c r="D7" t="str">
-        <v>B 304</v>
+        <v>A 1608</v>
       </c>
       <c r="E7" t="str">
         <v/>
       </c>
       <c r="F7" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G7">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H7" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I7" t="str">
         <v>PENDING</v>
       </c>
       <c r="J7" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K7" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L7" t="str">
+        <v/>
+      </c>
+      <c r="M7" t="str">
+        <v/>
+      </c>
+      <c r="N7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="str">
+        <v>2026-01-13 10:09</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Anuradha N</v>
+      </c>
+      <c r="D8" t="str">
+        <v>B 304</v>
+      </c>
+      <c r="E8" t="str">
+        <v/>
+      </c>
+      <c r="F8" t="str">
+        <v>Til Poli x1</v>
+      </c>
+      <c r="G8">
+        <v>30</v>
+      </c>
+      <c r="H8" t="str">
+        <v>COOKING</v>
+      </c>
+      <c r="I8" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J8" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K7" t="str">
+      <c r="K8" t="str">
         <v>16:45</v>
       </c>
-      <c r="L7" t="str">
-        <v/>
-      </c>
-      <c r="M7" t="str">
-        <v/>
-      </c>
-      <c r="N7" t="str">
+      <c r="L8" t="str">
+        <v/>
+      </c>
+      <c r="M8" t="str">
+        <v/>
+      </c>
+      <c r="N8" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N8"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -753,7 +797,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -762,13 +806,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>180</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-13.xlsx - 2026-01-13T18:59:43.619Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-13.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-13.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,25 +449,25 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 16:54</v>
+        <v>2026-01-13 18:59</v>
       </c>
       <c r="C2" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D2" t="str">
-        <v>a14</v>
+        <v>A-1608</v>
       </c>
       <c r="E2" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F2" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Jawar Bhakari x1</v>
       </c>
       <c r="G2">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -476,10 +476,10 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v/>
+        <v>2026-01-16</v>
       </c>
       <c r="K2" t="str">
-        <v/>
+        <v>10:00</v>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -493,16 +493,16 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 16:41</v>
+        <v>2026-01-13 16:54</v>
       </c>
       <c r="C3" t="str">
         <v>Pooja</v>
       </c>
       <c r="D3" t="str">
-        <v>saf</v>
+        <v>a14</v>
       </c>
       <c r="E3" t="str">
         <v>9096648553</v>
@@ -520,10 +520,10 @@
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v>2026-01-15</v>
+        <v/>
       </c>
       <c r="K3" t="str">
-        <v>10:12</v>
+        <v/>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -537,25 +537,25 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 16:40</v>
+        <v>2026-01-13 16:41</v>
       </c>
       <c r="C4" t="str">
-        <v>Sagar Borse</v>
+        <v>Pooja</v>
       </c>
       <c r="D4" t="str">
-        <v>A-1608</v>
+        <v>saf</v>
       </c>
       <c r="E4" t="str">
-        <v>7588930329</v>
+        <v>9096648553</v>
       </c>
       <c r="F4" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G4">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H4" t="str">
         <v>NEW</v>
@@ -564,10 +564,10 @@
         <v>PENDING</v>
       </c>
       <c r="J4" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K4" t="str">
-        <v>10:00</v>
+        <v>10:12</v>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -581,25 +581,25 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-13 16:39</v>
+        <v>2026-01-13 16:40</v>
       </c>
       <c r="C5" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D5" t="str">
-        <v>A1608</v>
+        <v>A-1608</v>
       </c>
       <c r="E5" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F5" t="str">
-        <v>Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G5">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H5" t="str">
         <v>NEW</v>
@@ -611,7 +611,7 @@
         <v>2026-01-14</v>
       </c>
       <c r="K5" t="str">
-        <v>22:09</v>
+        <v>10:00</v>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -625,25 +625,25 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-13 11:15</v>
+        <v>2026-01-13 16:39</v>
       </c>
       <c r="C6" t="str">
-        <v>Ajay Dwarkunde</v>
+        <v>Pooja</v>
       </c>
       <c r="D6" t="str">
-        <v>b-703</v>
+        <v>A1608</v>
       </c>
       <c r="E6" t="str">
-        <v>8087172173</v>
+        <v>9096648553</v>
       </c>
       <c r="F6" t="str">
-        <v>Pohe x1</v>
+        <v>Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G6">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H6" t="str">
         <v>NEW</v>
@@ -652,10 +652,10 @@
         <v>PENDING</v>
       </c>
       <c r="J6" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K6" t="str">
-        <v>18:50</v>
+        <v>22:09</v>
       </c>
       <c r="L6" t="str">
         <v/>
@@ -669,25 +669,25 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C7" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D7" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E7" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F7" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G7">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H7" t="str">
         <v>NEW</v>
@@ -699,7 +699,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K7" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L7" t="str">
         <v/>
@@ -713,51 +713,95 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-01-13 10:09</v>
+        <v>2026-01-13 10:20</v>
       </c>
       <c r="C8" t="str">
-        <v>Anuradha N</v>
+        <v>Pooja</v>
       </c>
       <c r="D8" t="str">
-        <v>B 304</v>
+        <v>A 1608</v>
       </c>
       <c r="E8" t="str">
         <v/>
       </c>
       <c r="F8" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G8">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H8" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I8" t="str">
         <v>PENDING</v>
       </c>
       <c r="J8" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K8" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L8" t="str">
+        <v/>
+      </c>
+      <c r="M8" t="str">
+        <v/>
+      </c>
+      <c r="N8" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="str">
+        <v>2026-01-13 10:09</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Anuradha N</v>
+      </c>
+      <c r="D9" t="str">
+        <v>B 304</v>
+      </c>
+      <c r="E9" t="str">
+        <v/>
+      </c>
+      <c r="F9" t="str">
+        <v>Til Poli x1</v>
+      </c>
+      <c r="G9">
+        <v>30</v>
+      </c>
+      <c r="H9" t="str">
+        <v>COOKING</v>
+      </c>
+      <c r="I9" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J9" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K8" t="str">
+      <c r="K9" t="str">
         <v>16:45</v>
       </c>
-      <c r="L8" t="str">
-        <v/>
-      </c>
-      <c r="M8" t="str">
-        <v/>
-      </c>
-      <c r="N8" t="str">
+      <c r="L9" t="str">
+        <v/>
+      </c>
+      <c r="M9" t="str">
+        <v/>
+      </c>
+      <c r="N9" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N9"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -797,7 +841,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -806,13 +850,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>195</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-13.xlsx - 2026-01-13T19:05:24.099Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-13.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-13.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,25 +449,25 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 18:59</v>
+        <v>2026-01-13 19:05</v>
       </c>
       <c r="C2" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D2" t="str">
-        <v>A-1608</v>
+        <v>A1608</v>
       </c>
       <c r="E2" t="str">
         <v>7588930329</v>
       </c>
       <c r="F2" t="str">
-        <v>Jawar Bhakari x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G2">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -476,10 +476,10 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-16</v>
+        <v>2026-01-26</v>
       </c>
       <c r="K2" t="str">
-        <v>10:00</v>
+        <v>10:35</v>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -493,25 +493,25 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 16:54</v>
+        <v>2026-01-13 18:59</v>
       </c>
       <c r="C3" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D3" t="str">
-        <v>a14</v>
+        <v>A-1608</v>
       </c>
       <c r="E3" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F3" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Jawar Bhakari x1</v>
       </c>
       <c r="G3">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H3" t="str">
         <v>NEW</v>
@@ -520,10 +520,10 @@
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v/>
+        <v>2026-01-16</v>
       </c>
       <c r="K3" t="str">
-        <v/>
+        <v>10:00</v>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -537,16 +537,16 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 16:41</v>
+        <v>2026-01-13 16:54</v>
       </c>
       <c r="C4" t="str">
         <v>Pooja</v>
       </c>
       <c r="D4" t="str">
-        <v>saf</v>
+        <v>a14</v>
       </c>
       <c r="E4" t="str">
         <v>9096648553</v>
@@ -564,10 +564,10 @@
         <v>PENDING</v>
       </c>
       <c r="J4" t="str">
-        <v>2026-01-15</v>
+        <v/>
       </c>
       <c r="K4" t="str">
-        <v>10:12</v>
+        <v/>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -581,25 +581,25 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-13 16:40</v>
+        <v>2026-01-13 16:41</v>
       </c>
       <c r="C5" t="str">
-        <v>Sagar Borse</v>
+        <v>Pooja</v>
       </c>
       <c r="D5" t="str">
-        <v>A-1608</v>
+        <v>saf</v>
       </c>
       <c r="E5" t="str">
-        <v>7588930329</v>
+        <v>9096648553</v>
       </c>
       <c r="F5" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G5">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H5" t="str">
         <v>NEW</v>
@@ -608,10 +608,10 @@
         <v>PENDING</v>
       </c>
       <c r="J5" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K5" t="str">
-        <v>10:00</v>
+        <v>10:12</v>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -625,25 +625,25 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-13 16:39</v>
+        <v>2026-01-13 16:40</v>
       </c>
       <c r="C6" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D6" t="str">
-        <v>A1608</v>
+        <v>A-1608</v>
       </c>
       <c r="E6" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F6" t="str">
-        <v>Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G6">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H6" t="str">
         <v>NEW</v>
@@ -655,7 +655,7 @@
         <v>2026-01-14</v>
       </c>
       <c r="K6" t="str">
-        <v>22:09</v>
+        <v>10:00</v>
       </c>
       <c r="L6" t="str">
         <v/>
@@ -669,25 +669,25 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-13 11:15</v>
+        <v>2026-01-13 16:39</v>
       </c>
       <c r="C7" t="str">
-        <v>Ajay Dwarkunde</v>
+        <v>Pooja</v>
       </c>
       <c r="D7" t="str">
-        <v>b-703</v>
+        <v>A1608</v>
       </c>
       <c r="E7" t="str">
-        <v>8087172173</v>
+        <v>9096648553</v>
       </c>
       <c r="F7" t="str">
-        <v>Pohe x1</v>
+        <v>Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G7">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H7" t="str">
         <v>NEW</v>
@@ -696,10 +696,10 @@
         <v>PENDING</v>
       </c>
       <c r="J7" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K7" t="str">
-        <v>18:50</v>
+        <v>22:09</v>
       </c>
       <c r="L7" t="str">
         <v/>
@@ -713,25 +713,25 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C8" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D8" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E8" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F8" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G8">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H8" t="str">
         <v>NEW</v>
@@ -743,7 +743,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K8" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L8" t="str">
         <v/>
@@ -757,51 +757,95 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" t="str">
-        <v>2026-01-13 10:09</v>
+        <v>2026-01-13 10:20</v>
       </c>
       <c r="C9" t="str">
-        <v>Anuradha N</v>
+        <v>Pooja</v>
       </c>
       <c r="D9" t="str">
-        <v>B 304</v>
+        <v>A 1608</v>
       </c>
       <c r="E9" t="str">
         <v/>
       </c>
       <c r="F9" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G9">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H9" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I9" t="str">
         <v>PENDING</v>
       </c>
       <c r="J9" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K9" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L9" t="str">
+        <v/>
+      </c>
+      <c r="M9" t="str">
+        <v/>
+      </c>
+      <c r="N9" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="str">
+        <v>2026-01-13 10:09</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Anuradha N</v>
+      </c>
+      <c r="D10" t="str">
+        <v>B 304</v>
+      </c>
+      <c r="E10" t="str">
+        <v/>
+      </c>
+      <c r="F10" t="str">
+        <v>Til Poli x1</v>
+      </c>
+      <c r="G10">
+        <v>30</v>
+      </c>
+      <c r="H10" t="str">
+        <v>COOKING</v>
+      </c>
+      <c r="I10" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J10" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K9" t="str">
+      <c r="K10" t="str">
         <v>16:45</v>
       </c>
-      <c r="L9" t="str">
-        <v/>
-      </c>
-      <c r="M9" t="str">
-        <v/>
-      </c>
-      <c r="N9" t="str">
+      <c r="L10" t="str">
+        <v/>
+      </c>
+      <c r="M10" t="str">
+        <v/>
+      </c>
+      <c r="N10" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N10"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -841,7 +885,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -850,13 +894,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>215</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-13.xlsx - 2026-01-13T19:12:11.013Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-13.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-13.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,16 +449,16 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 19:05</v>
+        <v>2026-01-13 19:12</v>
       </c>
       <c r="C2" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D2" t="str">
-        <v>A1608</v>
+        <v>Yuu</v>
       </c>
       <c r="E2" t="str">
         <v>7588930329</v>
@@ -470,16 +470,16 @@
         <v>15</v>
       </c>
       <c r="H2" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I2" t="str">
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-26</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K2" t="str">
-        <v>10:35</v>
+        <v>02:42</v>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -493,37 +493,37 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 18:59</v>
+        <v>2026-01-13 19:05</v>
       </c>
       <c r="C3" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D3" t="str">
-        <v>A-1608</v>
+        <v>A1608</v>
       </c>
       <c r="E3" t="str">
         <v>7588930329</v>
       </c>
       <c r="F3" t="str">
-        <v>Jawar Bhakari x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G3">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H3" t="str">
-        <v>NEW</v>
+        <v>COOKING</v>
       </c>
       <c r="I3" t="str">
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v>2026-01-16</v>
+        <v>2026-01-26</v>
       </c>
       <c r="K3" t="str">
-        <v>10:00</v>
+        <v>10:35</v>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -537,25 +537,25 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 16:54</v>
+        <v>2026-01-13 18:59</v>
       </c>
       <c r="C4" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D4" t="str">
-        <v>a14</v>
+        <v>A-1608</v>
       </c>
       <c r="E4" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F4" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Jawar Bhakari x1</v>
       </c>
       <c r="G4">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H4" t="str">
         <v>NEW</v>
@@ -564,10 +564,10 @@
         <v>PENDING</v>
       </c>
       <c r="J4" t="str">
-        <v/>
+        <v>2026-01-16</v>
       </c>
       <c r="K4" t="str">
-        <v/>
+        <v>10:00</v>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -581,16 +581,16 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-13 16:41</v>
+        <v>2026-01-13 16:54</v>
       </c>
       <c r="C5" t="str">
         <v>Pooja</v>
       </c>
       <c r="D5" t="str">
-        <v>saf</v>
+        <v>a14</v>
       </c>
       <c r="E5" t="str">
         <v>9096648553</v>
@@ -608,10 +608,10 @@
         <v>PENDING</v>
       </c>
       <c r="J5" t="str">
-        <v>2026-01-15</v>
+        <v/>
       </c>
       <c r="K5" t="str">
-        <v>10:12</v>
+        <v/>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -625,25 +625,25 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-13 16:40</v>
+        <v>2026-01-13 16:41</v>
       </c>
       <c r="C6" t="str">
-        <v>Sagar Borse</v>
+        <v>Pooja</v>
       </c>
       <c r="D6" t="str">
-        <v>A-1608</v>
+        <v>saf</v>
       </c>
       <c r="E6" t="str">
-        <v>7588930329</v>
+        <v>9096648553</v>
       </c>
       <c r="F6" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G6">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H6" t="str">
         <v>NEW</v>
@@ -652,10 +652,10 @@
         <v>PENDING</v>
       </c>
       <c r="J6" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K6" t="str">
-        <v>10:00</v>
+        <v>10:12</v>
       </c>
       <c r="L6" t="str">
         <v/>
@@ -669,25 +669,25 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-13 16:39</v>
+        <v>2026-01-13 16:40</v>
       </c>
       <c r="C7" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D7" t="str">
-        <v>A1608</v>
+        <v>A-1608</v>
       </c>
       <c r="E7" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F7" t="str">
-        <v>Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G7">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H7" t="str">
         <v>NEW</v>
@@ -699,7 +699,7 @@
         <v>2026-01-14</v>
       </c>
       <c r="K7" t="str">
-        <v>22:09</v>
+        <v>10:00</v>
       </c>
       <c r="L7" t="str">
         <v/>
@@ -713,25 +713,25 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-01-13 11:15</v>
+        <v>2026-01-13 16:39</v>
       </c>
       <c r="C8" t="str">
-        <v>Ajay Dwarkunde</v>
+        <v>Pooja</v>
       </c>
       <c r="D8" t="str">
-        <v>b-703</v>
+        <v>A1608</v>
       </c>
       <c r="E8" t="str">
-        <v>8087172173</v>
+        <v>9096648553</v>
       </c>
       <c r="F8" t="str">
-        <v>Pohe x1</v>
+        <v>Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G8">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H8" t="str">
         <v>NEW</v>
@@ -740,10 +740,10 @@
         <v>PENDING</v>
       </c>
       <c r="J8" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K8" t="str">
-        <v>18:50</v>
+        <v>22:09</v>
       </c>
       <c r="L8" t="str">
         <v/>
@@ -757,25 +757,25 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C9" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D9" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E9" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F9" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G9">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H9" t="str">
         <v>NEW</v>
@@ -787,7 +787,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K9" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L9" t="str">
         <v/>
@@ -801,51 +801,95 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" t="str">
-        <v>2026-01-13 10:09</v>
+        <v>2026-01-13 10:20</v>
       </c>
       <c r="C10" t="str">
-        <v>Anuradha N</v>
+        <v>Pooja</v>
       </c>
       <c r="D10" t="str">
-        <v>B 304</v>
+        <v>A 1608</v>
       </c>
       <c r="E10" t="str">
         <v/>
       </c>
       <c r="F10" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G10">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H10" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I10" t="str">
         <v>PENDING</v>
       </c>
       <c r="J10" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K10" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L10" t="str">
+        <v/>
+      </c>
+      <c r="M10" t="str">
+        <v/>
+      </c>
+      <c r="N10" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="str">
+        <v>2026-01-13 10:09</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Anuradha N</v>
+      </c>
+      <c r="D11" t="str">
+        <v>B 304</v>
+      </c>
+      <c r="E11" t="str">
+        <v/>
+      </c>
+      <c r="F11" t="str">
+        <v>Til Poli x1</v>
+      </c>
+      <c r="G11">
+        <v>30</v>
+      </c>
+      <c r="H11" t="str">
+        <v>COOKING</v>
+      </c>
+      <c r="I11" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J11" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K10" t="str">
+      <c r="K11" t="str">
         <v>16:45</v>
       </c>
-      <c r="L10" t="str">
-        <v/>
-      </c>
-      <c r="M10" t="str">
-        <v/>
-      </c>
-      <c r="N10" t="str">
+      <c r="L11" t="str">
+        <v/>
+      </c>
+      <c r="M11" t="str">
+        <v/>
+      </c>
+      <c r="N11" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N11"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -885,7 +929,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="B2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -894,13 +938,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>230</v>
+        <v>245</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>230</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-13.xlsx - 2026-01-13T22:38:59.403Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-13.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-13.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,25 +449,25 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 19:12</v>
+        <v>2026-01-13 22:38</v>
       </c>
       <c r="C2" t="str">
-        <v>Sagar Borse</v>
+        <v>Phantom</v>
       </c>
       <c r="D2" t="str">
-        <v>Yuu</v>
+        <v>420</v>
       </c>
       <c r="E2" t="str">
-        <v>7588930329</v>
+        <v/>
       </c>
       <c r="F2" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Upma x1</v>
       </c>
       <c r="G2">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -476,10 +476,10 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-15</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K2" t="str">
-        <v>02:42</v>
+        <v>15:38</v>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -493,16 +493,16 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 19:05</v>
+        <v>2026-01-13 19:12</v>
       </c>
       <c r="C3" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D3" t="str">
-        <v>A1608</v>
+        <v>Yuu</v>
       </c>
       <c r="E3" t="str">
         <v>7588930329</v>
@@ -514,16 +514,16 @@
         <v>15</v>
       </c>
       <c r="H3" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I3" t="str">
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v>2026-01-26</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K3" t="str">
-        <v>10:35</v>
+        <v>02:42</v>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -537,37 +537,37 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 18:59</v>
+        <v>2026-01-13 19:05</v>
       </c>
       <c r="C4" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D4" t="str">
-        <v>A-1608</v>
+        <v>A1608</v>
       </c>
       <c r="E4" t="str">
         <v>7588930329</v>
       </c>
       <c r="F4" t="str">
-        <v>Jawar Bhakari x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G4">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H4" t="str">
-        <v>NEW</v>
+        <v>COOKING</v>
       </c>
       <c r="I4" t="str">
         <v>PENDING</v>
       </c>
       <c r="J4" t="str">
-        <v>2026-01-16</v>
+        <v>2026-01-26</v>
       </c>
       <c r="K4" t="str">
-        <v>10:00</v>
+        <v>10:35</v>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -581,25 +581,25 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-13 16:54</v>
+        <v>2026-01-13 18:59</v>
       </c>
       <c r="C5" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D5" t="str">
-        <v>a14</v>
+        <v>A-1608</v>
       </c>
       <c r="E5" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F5" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Jawar Bhakari x1</v>
       </c>
       <c r="G5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H5" t="str">
         <v>NEW</v>
@@ -608,10 +608,10 @@
         <v>PENDING</v>
       </c>
       <c r="J5" t="str">
-        <v/>
+        <v>2026-01-16</v>
       </c>
       <c r="K5" t="str">
-        <v/>
+        <v>10:00</v>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -625,16 +625,16 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-13 16:41</v>
+        <v>2026-01-13 16:54</v>
       </c>
       <c r="C6" t="str">
         <v>Pooja</v>
       </c>
       <c r="D6" t="str">
-        <v>saf</v>
+        <v>a14</v>
       </c>
       <c r="E6" t="str">
         <v>9096648553</v>
@@ -652,10 +652,10 @@
         <v>PENDING</v>
       </c>
       <c r="J6" t="str">
-        <v>2026-01-15</v>
+        <v/>
       </c>
       <c r="K6" t="str">
-        <v>10:12</v>
+        <v/>
       </c>
       <c r="L6" t="str">
         <v/>
@@ -669,25 +669,25 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-13 16:40</v>
+        <v>2026-01-13 16:41</v>
       </c>
       <c r="C7" t="str">
-        <v>Sagar Borse</v>
+        <v>Pooja</v>
       </c>
       <c r="D7" t="str">
-        <v>A-1608</v>
+        <v>saf</v>
       </c>
       <c r="E7" t="str">
-        <v>7588930329</v>
+        <v>9096648553</v>
       </c>
       <c r="F7" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G7">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H7" t="str">
         <v>NEW</v>
@@ -696,10 +696,10 @@
         <v>PENDING</v>
       </c>
       <c r="J7" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K7" t="str">
-        <v>10:00</v>
+        <v>10:12</v>
       </c>
       <c r="L7" t="str">
         <v/>
@@ -713,25 +713,25 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-01-13 16:39</v>
+        <v>2026-01-13 16:40</v>
       </c>
       <c r="C8" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D8" t="str">
-        <v>A1608</v>
+        <v>A-1608</v>
       </c>
       <c r="E8" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F8" t="str">
-        <v>Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G8">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H8" t="str">
         <v>NEW</v>
@@ -743,7 +743,7 @@
         <v>2026-01-14</v>
       </c>
       <c r="K8" t="str">
-        <v>22:09</v>
+        <v>10:00</v>
       </c>
       <c r="L8" t="str">
         <v/>
@@ -757,25 +757,25 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9" t="str">
-        <v>2026-01-13 11:15</v>
+        <v>2026-01-13 16:39</v>
       </c>
       <c r="C9" t="str">
-        <v>Ajay Dwarkunde</v>
+        <v>Pooja</v>
       </c>
       <c r="D9" t="str">
-        <v>b-703</v>
+        <v>A1608</v>
       </c>
       <c r="E9" t="str">
-        <v>8087172173</v>
+        <v>9096648553</v>
       </c>
       <c r="F9" t="str">
-        <v>Pohe x1</v>
+        <v>Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G9">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H9" t="str">
         <v>NEW</v>
@@ -784,10 +784,10 @@
         <v>PENDING</v>
       </c>
       <c r="J9" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K9" t="str">
-        <v>18:50</v>
+        <v>22:09</v>
       </c>
       <c r="L9" t="str">
         <v/>
@@ -801,25 +801,25 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B10" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C10" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D10" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E10" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F10" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G10">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H10" t="str">
         <v>NEW</v>
@@ -831,7 +831,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K10" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L10" t="str">
         <v/>
@@ -845,51 +845,95 @@
     </row>
     <row r="11">
       <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="str">
+        <v>2026-01-13 10:20</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D11" t="str">
+        <v>A 1608</v>
+      </c>
+      <c r="E11" t="str">
+        <v/>
+      </c>
+      <c r="F11" t="str">
+        <v>Wheat Chapati x1</v>
+      </c>
+      <c r="G11">
+        <v>15</v>
+      </c>
+      <c r="H11" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I11" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J11" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K11" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L11" t="str">
+        <v/>
+      </c>
+      <c r="M11" t="str">
+        <v/>
+      </c>
+      <c r="N11" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
         <v>1</v>
       </c>
-      <c r="B11" t="str">
+      <c r="B12" t="str">
         <v>2026-01-13 10:09</v>
       </c>
-      <c r="C11" t="str">
+      <c r="C12" t="str">
         <v>Anuradha N</v>
       </c>
-      <c r="D11" t="str">
+      <c r="D12" t="str">
         <v>B 304</v>
       </c>
-      <c r="E11" t="str">
-        <v/>
-      </c>
-      <c r="F11" t="str">
+      <c r="E12" t="str">
+        <v/>
+      </c>
+      <c r="F12" t="str">
         <v>Til Poli x1</v>
       </c>
-      <c r="G11">
+      <c r="G12">
         <v>30</v>
       </c>
-      <c r="H11" t="str">
+      <c r="H12" t="str">
         <v>COOKING</v>
       </c>
-      <c r="I11" t="str">
-        <v>PENDING</v>
-      </c>
-      <c r="J11" t="str">
+      <c r="I12" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J12" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K11" t="str">
+      <c r="K12" t="str">
         <v>16:45</v>
       </c>
-      <c r="L11" t="str">
-        <v/>
-      </c>
-      <c r="M11" t="str">
-        <v/>
-      </c>
-      <c r="N11" t="str">
+      <c r="L12" t="str">
+        <v/>
+      </c>
+      <c r="M12" t="str">
+        <v/>
+      </c>
+      <c r="N12" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N12"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -929,7 +973,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -938,13 +982,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>245</v>
+        <v>275</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>245</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-13.xlsx - 2026-01-13T22:43:08.654Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-13.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-13.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,13 +449,13 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 22:38</v>
+        <v>2026-01-13 22:43</v>
       </c>
       <c r="C2" t="str">
-        <v>Phantom</v>
+        <v>Swapnil (Phantom)</v>
       </c>
       <c r="D2" t="str">
         <v>420</v>
@@ -464,10 +464,10 @@
         <v/>
       </c>
       <c r="F2" t="str">
-        <v>Upma x1</v>
+        <v>Vermicelli Kheer x1</v>
       </c>
       <c r="G2">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -476,13 +476,13 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K2" t="str">
-        <v>15:38</v>
+        <v>16:42</v>
       </c>
       <c r="L2" t="str">
-        <v/>
+        <v>No vermicelli in kheer please.</v>
       </c>
       <c r="M2" t="str">
         <v/>
@@ -493,25 +493,25 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 19:12</v>
+        <v>2026-01-13 22:38</v>
       </c>
       <c r="C3" t="str">
-        <v>Sagar Borse</v>
+        <v>Phantom</v>
       </c>
       <c r="D3" t="str">
-        <v>Yuu</v>
+        <v>420</v>
       </c>
       <c r="E3" t="str">
-        <v>7588930329</v>
+        <v/>
       </c>
       <c r="F3" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Upma x1</v>
       </c>
       <c r="G3">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H3" t="str">
         <v>NEW</v>
@@ -520,10 +520,10 @@
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v>2026-01-15</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K3" t="str">
-        <v>02:42</v>
+        <v>15:38</v>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -537,16 +537,16 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 19:05</v>
+        <v>2026-01-13 19:12</v>
       </c>
       <c r="C4" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D4" t="str">
-        <v>A1608</v>
+        <v>Yuu</v>
       </c>
       <c r="E4" t="str">
         <v>7588930329</v>
@@ -558,16 +558,16 @@
         <v>15</v>
       </c>
       <c r="H4" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I4" t="str">
         <v>PENDING</v>
       </c>
       <c r="J4" t="str">
-        <v>2026-01-26</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K4" t="str">
-        <v>10:35</v>
+        <v>02:42</v>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -581,37 +581,37 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-13 18:59</v>
+        <v>2026-01-13 19:05</v>
       </c>
       <c r="C5" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D5" t="str">
-        <v>A-1608</v>
+        <v>A1608</v>
       </c>
       <c r="E5" t="str">
         <v>7588930329</v>
       </c>
       <c r="F5" t="str">
-        <v>Jawar Bhakari x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G5">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H5" t="str">
-        <v>NEW</v>
+        <v>COOKING</v>
       </c>
       <c r="I5" t="str">
         <v>PENDING</v>
       </c>
       <c r="J5" t="str">
-        <v>2026-01-16</v>
+        <v>2026-01-26</v>
       </c>
       <c r="K5" t="str">
-        <v>10:00</v>
+        <v>10:35</v>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -625,25 +625,25 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-13 16:54</v>
+        <v>2026-01-13 18:59</v>
       </c>
       <c r="C6" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D6" t="str">
-        <v>a14</v>
+        <v>A-1608</v>
       </c>
       <c r="E6" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F6" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Jawar Bhakari x1</v>
       </c>
       <c r="G6">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H6" t="str">
         <v>NEW</v>
@@ -652,10 +652,10 @@
         <v>PENDING</v>
       </c>
       <c r="J6" t="str">
-        <v/>
+        <v>2026-01-16</v>
       </c>
       <c r="K6" t="str">
-        <v/>
+        <v>10:00</v>
       </c>
       <c r="L6" t="str">
         <v/>
@@ -669,16 +669,16 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-13 16:41</v>
+        <v>2026-01-13 16:54</v>
       </c>
       <c r="C7" t="str">
         <v>Pooja</v>
       </c>
       <c r="D7" t="str">
-        <v>saf</v>
+        <v>a14</v>
       </c>
       <c r="E7" t="str">
         <v>9096648553</v>
@@ -696,10 +696,10 @@
         <v>PENDING</v>
       </c>
       <c r="J7" t="str">
-        <v>2026-01-15</v>
+        <v/>
       </c>
       <c r="K7" t="str">
-        <v>10:12</v>
+        <v/>
       </c>
       <c r="L7" t="str">
         <v/>
@@ -713,25 +713,25 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-01-13 16:40</v>
+        <v>2026-01-13 16:41</v>
       </c>
       <c r="C8" t="str">
-        <v>Sagar Borse</v>
+        <v>Pooja</v>
       </c>
       <c r="D8" t="str">
-        <v>A-1608</v>
+        <v>saf</v>
       </c>
       <c r="E8" t="str">
-        <v>7588930329</v>
+        <v>9096648553</v>
       </c>
       <c r="F8" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G8">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H8" t="str">
         <v>NEW</v>
@@ -740,10 +740,10 @@
         <v>PENDING</v>
       </c>
       <c r="J8" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K8" t="str">
-        <v>10:00</v>
+        <v>10:12</v>
       </c>
       <c r="L8" t="str">
         <v/>
@@ -757,25 +757,25 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" t="str">
-        <v>2026-01-13 16:39</v>
+        <v>2026-01-13 16:40</v>
       </c>
       <c r="C9" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D9" t="str">
-        <v>A1608</v>
+        <v>A-1608</v>
       </c>
       <c r="E9" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F9" t="str">
-        <v>Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G9">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H9" t="str">
         <v>NEW</v>
@@ -787,7 +787,7 @@
         <v>2026-01-14</v>
       </c>
       <c r="K9" t="str">
-        <v>22:09</v>
+        <v>10:00</v>
       </c>
       <c r="L9" t="str">
         <v/>
@@ -801,25 +801,25 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B10" t="str">
-        <v>2026-01-13 11:15</v>
+        <v>2026-01-13 16:39</v>
       </c>
       <c r="C10" t="str">
-        <v>Ajay Dwarkunde</v>
+        <v>Pooja</v>
       </c>
       <c r="D10" t="str">
-        <v>b-703</v>
+        <v>A1608</v>
       </c>
       <c r="E10" t="str">
-        <v>8087172173</v>
+        <v>9096648553</v>
       </c>
       <c r="F10" t="str">
-        <v>Pohe x1</v>
+        <v>Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G10">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H10" t="str">
         <v>NEW</v>
@@ -828,10 +828,10 @@
         <v>PENDING</v>
       </c>
       <c r="J10" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K10" t="str">
-        <v>18:50</v>
+        <v>22:09</v>
       </c>
       <c r="L10" t="str">
         <v/>
@@ -845,25 +845,25 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B11" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C11" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D11" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E11" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F11" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G11">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H11" t="str">
         <v>NEW</v>
@@ -875,7 +875,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K11" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L11" t="str">
         <v/>
@@ -889,51 +889,95 @@
     </row>
     <row r="12">
       <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="str">
+        <v>2026-01-13 10:20</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D12" t="str">
+        <v>A 1608</v>
+      </c>
+      <c r="E12" t="str">
+        <v/>
+      </c>
+      <c r="F12" t="str">
+        <v>Wheat Chapati x1</v>
+      </c>
+      <c r="G12">
+        <v>15</v>
+      </c>
+      <c r="H12" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I12" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J12" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K12" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L12" t="str">
+        <v/>
+      </c>
+      <c r="M12" t="str">
+        <v/>
+      </c>
+      <c r="N12" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
         <v>1</v>
       </c>
-      <c r="B12" t="str">
+      <c r="B13" t="str">
         <v>2026-01-13 10:09</v>
       </c>
-      <c r="C12" t="str">
+      <c r="C13" t="str">
         <v>Anuradha N</v>
       </c>
-      <c r="D12" t="str">
+      <c r="D13" t="str">
         <v>B 304</v>
       </c>
-      <c r="E12" t="str">
-        <v/>
-      </c>
-      <c r="F12" t="str">
+      <c r="E13" t="str">
+        <v/>
+      </c>
+      <c r="F13" t="str">
         <v>Til Poli x1</v>
       </c>
-      <c r="G12">
+      <c r="G13">
         <v>30</v>
       </c>
-      <c r="H12" t="str">
+      <c r="H13" t="str">
         <v>COOKING</v>
       </c>
-      <c r="I12" t="str">
-        <v>PENDING</v>
-      </c>
-      <c r="J12" t="str">
+      <c r="I13" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J13" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K12" t="str">
+      <c r="K13" t="str">
         <v>16:45</v>
       </c>
-      <c r="L12" t="str">
-        <v/>
-      </c>
-      <c r="M12" t="str">
-        <v/>
-      </c>
-      <c r="N12" t="str">
+      <c r="L13" t="str">
+        <v/>
+      </c>
+      <c r="M13" t="str">
+        <v/>
+      </c>
+      <c r="N13" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N13"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -973,7 +1017,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="B2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -982,13 +1026,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>275</v>
+        <v>325</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>275</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-13.xlsx - 2026-01-13T22:51:30.465Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-13.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-13.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,25 +449,25 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 22:43</v>
+        <v>2026-01-13 22:51</v>
       </c>
       <c r="C2" t="str">
-        <v>Swapnil (Phantom)</v>
+        <v>Ketki</v>
       </c>
       <c r="D2" t="str">
-        <v>420</v>
+        <v>1608</v>
       </c>
       <c r="E2" t="str">
-        <v/>
+        <v>3159135521</v>
       </c>
       <c r="F2" t="str">
-        <v>Vermicelli Kheer x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G2">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -476,13 +476,13 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-15</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K2" t="str">
-        <v>16:42</v>
+        <v>16:51</v>
       </c>
       <c r="L2" t="str">
-        <v>No vermicelli in kheer please.</v>
+        <v/>
       </c>
       <c r="M2" t="str">
         <v/>
@@ -493,13 +493,13 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 22:38</v>
+        <v>2026-01-13 22:43</v>
       </c>
       <c r="C3" t="str">
-        <v>Phantom</v>
+        <v>Swapnil (Phantom)</v>
       </c>
       <c r="D3" t="str">
         <v>420</v>
@@ -508,10 +508,10 @@
         <v/>
       </c>
       <c r="F3" t="str">
-        <v>Upma x1</v>
+        <v>Vermicelli Kheer x1</v>
       </c>
       <c r="G3">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H3" t="str">
         <v>NEW</v>
@@ -520,13 +520,13 @@
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K3" t="str">
-        <v>15:38</v>
+        <v>16:42</v>
       </c>
       <c r="L3" t="str">
-        <v/>
+        <v>No vermicelli in kheer please.</v>
       </c>
       <c r="M3" t="str">
         <v/>
@@ -537,25 +537,25 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 19:12</v>
+        <v>2026-01-13 22:38</v>
       </c>
       <c r="C4" t="str">
-        <v>Sagar Borse</v>
+        <v>Phantom</v>
       </c>
       <c r="D4" t="str">
-        <v>Yuu</v>
+        <v>420</v>
       </c>
       <c r="E4" t="str">
-        <v>7588930329</v>
+        <v/>
       </c>
       <c r="F4" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Upma x1</v>
       </c>
       <c r="G4">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H4" t="str">
         <v>NEW</v>
@@ -564,10 +564,10 @@
         <v>PENDING</v>
       </c>
       <c r="J4" t="str">
-        <v>2026-01-15</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K4" t="str">
-        <v>02:42</v>
+        <v>15:38</v>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -581,16 +581,16 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-13 19:05</v>
+        <v>2026-01-13 19:12</v>
       </c>
       <c r="C5" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D5" t="str">
-        <v>A1608</v>
+        <v>Yuu</v>
       </c>
       <c r="E5" t="str">
         <v>7588930329</v>
@@ -602,16 +602,16 @@
         <v>15</v>
       </c>
       <c r="H5" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I5" t="str">
         <v>PENDING</v>
       </c>
       <c r="J5" t="str">
-        <v>2026-01-26</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K5" t="str">
-        <v>10:35</v>
+        <v>02:42</v>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -625,37 +625,37 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-13 18:59</v>
+        <v>2026-01-13 19:05</v>
       </c>
       <c r="C6" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D6" t="str">
-        <v>A-1608</v>
+        <v>A1608</v>
       </c>
       <c r="E6" t="str">
         <v>7588930329</v>
       </c>
       <c r="F6" t="str">
-        <v>Jawar Bhakari x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G6">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H6" t="str">
-        <v>NEW</v>
+        <v>COOKING</v>
       </c>
       <c r="I6" t="str">
         <v>PENDING</v>
       </c>
       <c r="J6" t="str">
-        <v>2026-01-16</v>
+        <v>2026-01-26</v>
       </c>
       <c r="K6" t="str">
-        <v>10:00</v>
+        <v>10:35</v>
       </c>
       <c r="L6" t="str">
         <v/>
@@ -669,25 +669,25 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-13 16:54</v>
+        <v>2026-01-13 18:59</v>
       </c>
       <c r="C7" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D7" t="str">
-        <v>a14</v>
+        <v>A-1608</v>
       </c>
       <c r="E7" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F7" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Jawar Bhakari x1</v>
       </c>
       <c r="G7">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H7" t="str">
         <v>NEW</v>
@@ -696,10 +696,10 @@
         <v>PENDING</v>
       </c>
       <c r="J7" t="str">
-        <v/>
+        <v>2026-01-16</v>
       </c>
       <c r="K7" t="str">
-        <v/>
+        <v>10:00</v>
       </c>
       <c r="L7" t="str">
         <v/>
@@ -713,16 +713,16 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-01-13 16:41</v>
+        <v>2026-01-13 16:54</v>
       </c>
       <c r="C8" t="str">
         <v>Pooja</v>
       </c>
       <c r="D8" t="str">
-        <v>saf</v>
+        <v>a14</v>
       </c>
       <c r="E8" t="str">
         <v>9096648553</v>
@@ -740,10 +740,10 @@
         <v>PENDING</v>
       </c>
       <c r="J8" t="str">
-        <v>2026-01-15</v>
+        <v/>
       </c>
       <c r="K8" t="str">
-        <v>10:12</v>
+        <v/>
       </c>
       <c r="L8" t="str">
         <v/>
@@ -757,25 +757,25 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" t="str">
-        <v>2026-01-13 16:40</v>
+        <v>2026-01-13 16:41</v>
       </c>
       <c r="C9" t="str">
-        <v>Sagar Borse</v>
+        <v>Pooja</v>
       </c>
       <c r="D9" t="str">
-        <v>A-1608</v>
+        <v>saf</v>
       </c>
       <c r="E9" t="str">
-        <v>7588930329</v>
+        <v>9096648553</v>
       </c>
       <c r="F9" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G9">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H9" t="str">
         <v>NEW</v>
@@ -784,10 +784,10 @@
         <v>PENDING</v>
       </c>
       <c r="J9" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K9" t="str">
-        <v>10:00</v>
+        <v>10:12</v>
       </c>
       <c r="L9" t="str">
         <v/>
@@ -801,25 +801,25 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10" t="str">
-        <v>2026-01-13 16:39</v>
+        <v>2026-01-13 16:40</v>
       </c>
       <c r="C10" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D10" t="str">
-        <v>A1608</v>
+        <v>A-1608</v>
       </c>
       <c r="E10" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F10" t="str">
-        <v>Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G10">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H10" t="str">
         <v>NEW</v>
@@ -831,7 +831,7 @@
         <v>2026-01-14</v>
       </c>
       <c r="K10" t="str">
-        <v>22:09</v>
+        <v>10:00</v>
       </c>
       <c r="L10" t="str">
         <v/>
@@ -845,25 +845,25 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B11" t="str">
-        <v>2026-01-13 11:15</v>
+        <v>2026-01-13 16:39</v>
       </c>
       <c r="C11" t="str">
-        <v>Ajay Dwarkunde</v>
+        <v>Pooja</v>
       </c>
       <c r="D11" t="str">
-        <v>b-703</v>
+        <v>A1608</v>
       </c>
       <c r="E11" t="str">
-        <v>8087172173</v>
+        <v>9096648553</v>
       </c>
       <c r="F11" t="str">
-        <v>Pohe x1</v>
+        <v>Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G11">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H11" t="str">
         <v>NEW</v>
@@ -872,10 +872,10 @@
         <v>PENDING</v>
       </c>
       <c r="J11" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K11" t="str">
-        <v>18:50</v>
+        <v>22:09</v>
       </c>
       <c r="L11" t="str">
         <v/>
@@ -889,25 +889,25 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B12" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C12" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D12" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E12" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F12" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G12">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H12" t="str">
         <v>NEW</v>
@@ -919,7 +919,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K12" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L12" t="str">
         <v/>
@@ -933,51 +933,95 @@
     </row>
     <row r="13">
       <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="str">
+        <v>2026-01-13 10:20</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D13" t="str">
+        <v>A 1608</v>
+      </c>
+      <c r="E13" t="str">
+        <v/>
+      </c>
+      <c r="F13" t="str">
+        <v>Wheat Chapati x1</v>
+      </c>
+      <c r="G13">
+        <v>15</v>
+      </c>
+      <c r="H13" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I13" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J13" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K13" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L13" t="str">
+        <v/>
+      </c>
+      <c r="M13" t="str">
+        <v/>
+      </c>
+      <c r="N13" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
         <v>1</v>
       </c>
-      <c r="B13" t="str">
+      <c r="B14" t="str">
         <v>2026-01-13 10:09</v>
       </c>
-      <c r="C13" t="str">
+      <c r="C14" t="str">
         <v>Anuradha N</v>
       </c>
-      <c r="D13" t="str">
+      <c r="D14" t="str">
         <v>B 304</v>
       </c>
-      <c r="E13" t="str">
-        <v/>
-      </c>
-      <c r="F13" t="str">
+      <c r="E14" t="str">
+        <v/>
+      </c>
+      <c r="F14" t="str">
         <v>Til Poli x1</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <v>30</v>
       </c>
-      <c r="H13" t="str">
+      <c r="H14" t="str">
         <v>COOKING</v>
       </c>
-      <c r="I13" t="str">
-        <v>PENDING</v>
-      </c>
-      <c r="J13" t="str">
+      <c r="I14" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J14" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K13" t="str">
+      <c r="K14" t="str">
         <v>16:45</v>
       </c>
-      <c r="L13" t="str">
-        <v/>
-      </c>
-      <c r="M13" t="str">
-        <v/>
-      </c>
-      <c r="N13" t="str">
+      <c r="L14" t="str">
+        <v/>
+      </c>
+      <c r="M14" t="str">
+        <v/>
+      </c>
+      <c r="N14" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N13"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N14"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1017,7 +1061,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="B2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1026,13 +1070,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>325</v>
+        <v>340</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>325</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>